<commit_message>
Small changes to LC and OT
</commit_message>
<xml_diff>
--- a/P3/Results/Data/Spinat/AllOTResults.xlsx
+++ b/P3/Results/Data/Spinat/AllOTResults.xlsx
@@ -6,7 +6,13 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Spinach20g" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Spinach30g" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Spinach40g" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Spinach80g" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Spinach120g" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Spinach160g" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Spinach595g" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Spinach20g" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -412,9 +418,1474 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="65" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_20242011_094437.png</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="C2" t="n">
+        <v>14.52</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5.32</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5.37</v>
+      </c>
+      <c r="F2" t="n">
+        <v>20.66</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H2" t="n">
+        <v>4.23</v>
+      </c>
+      <c r="I2" t="n">
+        <v>15.28</v>
+      </c>
+      <c r="J2" t="n">
+        <v>5.11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp49690.0_20242011_102755.png</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>13.16</v>
+      </c>
+      <c r="C3" t="n">
+        <v>14.97</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-21.99</v>
+      </c>
+      <c r="E3" t="n">
+        <v>7.39</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10.84</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H3" t="n">
+        <v>8</v>
+      </c>
+      <c r="I3" t="n">
+        <v>10.67</v>
+      </c>
+      <c r="J3" t="n">
+        <v>9.18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_20242011_094451.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp38209.0_20242011_102820.png</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="C5" t="n">
+        <v>14.38</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5.44</v>
+      </c>
+      <c r="F5" t="n">
+        <v>19.68</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="I5" t="n">
+        <v>14.38</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_20242011_094542.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Infront_Camera_light10_exp22577.0_20242011_103029.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_20242011_094606.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Infront_Camera_light5_exp34813.0_20242011_103039.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_20242011_094522.png</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>11.61</v>
+      </c>
+      <c r="C10" t="n">
+        <v>14.64</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-7.3</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F10" t="n">
+        <v>17.81</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H10" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="I10" t="n">
+        <v>15.96</v>
+      </c>
+      <c r="J10" t="n">
+        <v>6.47</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp22577.0_20242011_102908.png</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>12.32</v>
+      </c>
+      <c r="C11" t="n">
+        <v>14.29</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-4.2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="F11" t="n">
+        <v>17.6</v>
+      </c>
+      <c r="G11" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H11" t="n">
+        <v>6.49</v>
+      </c>
+      <c r="I11" t="n">
+        <v>14.11</v>
+      </c>
+      <c r="J11" t="n">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_20242011_094508.png</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>8.91</v>
+      </c>
+      <c r="C12" t="n">
+        <v>12.98</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5.72</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F12" t="n">
+        <v>21.23</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H12" t="n">
+        <v>4.17</v>
+      </c>
+      <c r="I12" t="n">
+        <v>19.07</v>
+      </c>
+      <c r="J12" t="n">
+        <v>4.76</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp29370.0_20242011_102846.png</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>10.74</v>
+      </c>
+      <c r="C13" t="n">
+        <v>14.59</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.63</v>
+      </c>
+      <c r="F13" t="n">
+        <v>19.68</v>
+      </c>
+      <c r="G13" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H13" t="n">
+        <v>5.35</v>
+      </c>
+      <c r="I13" t="n">
+        <v>15.51</v>
+      </c>
+      <c r="J13" t="n">
+        <v>5.77</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp254895.0_20242011_103129.png</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>11.86</v>
+      </c>
+      <c r="C14" t="n">
+        <v>14.19</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-6.65</v>
+      </c>
+      <c r="E14" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="F14" t="n">
+        <v>18.01</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H14" t="n">
+        <v>6.08</v>
+      </c>
+      <c r="I14" t="n">
+        <v>13.87</v>
+      </c>
+      <c r="J14" t="n">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <f>COUNT(B2:B14)</f>
+        <v/>
+      </c>
+      <c r="B15">
+        <f>AVERAGE(B2:B14)</f>
+        <v/>
+      </c>
+      <c r="C15">
+        <f>AVERAGE(C2:C14)</f>
+        <v/>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(D2:D14)</f>
+        <v/>
+      </c>
+      <c r="E15">
+        <f>AVERAGE(E2:E14)</f>
+        <v/>
+      </c>
+      <c r="F15">
+        <f>AVERAGE(F2:F14)</f>
+        <v/>
+      </c>
+      <c r="G15">
+        <f>AVERAGE(G2:G14)</f>
+        <v/>
+      </c>
+      <c r="H15">
+        <f>AVERAGE(H2:H14)</f>
+        <v/>
+      </c>
+      <c r="I15">
+        <f>AVERAGE(I2:I14)</f>
+        <v/>
+      </c>
+      <c r="J15">
+        <f>AVERAGE(J2:J14)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="55" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp51537.0_20242011_124148.png</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>12.66</v>
+      </c>
+      <c r="C2" t="n">
+        <v>15.1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-19.71</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2.55</v>
+      </c>
+      <c r="F2" t="n">
+        <v>15.56</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H2" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="I2" t="n">
+        <v>12.62</v>
+      </c>
+      <c r="J2" t="n">
+        <v>7.14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp85960.0_20242011_124243.png</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>13.53</v>
+      </c>
+      <c r="C3" t="n">
+        <v>15.47</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-21.61</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4.01</v>
+      </c>
+      <c r="F3" t="n">
+        <v>14.85</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H3" t="n">
+        <v>6.38</v>
+      </c>
+      <c r="I3" t="n">
+        <v>12.52</v>
+      </c>
+      <c r="J3" t="n">
+        <v>7.92</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp24007.0_20242011_124516.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp41467.0_20242011_124606.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp28774.0_20242011_124414.png</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>12.41</v>
+      </c>
+      <c r="C6" t="n">
+        <v>15.38</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-20.62</v>
+      </c>
+      <c r="E6" t="n">
+        <v>7.73</v>
+      </c>
+      <c r="F6" t="n">
+        <v>12.83</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H6" t="n">
+        <v>7.04</v>
+      </c>
+      <c r="I6" t="n">
+        <v>10.66</v>
+      </c>
+      <c r="J6" t="n">
+        <v>8.699999999999999</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp49889.0_20242011_124336.png</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>13.39</v>
+      </c>
+      <c r="C7" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-15.45</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8.24</v>
+      </c>
+      <c r="F7" t="n">
+        <v>14.48</v>
+      </c>
+      <c r="G7" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H7" t="n">
+        <v>7.01</v>
+      </c>
+      <c r="I7" t="n">
+        <v>10.94</v>
+      </c>
+      <c r="J7" t="n">
+        <v>8.43</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <f>COUNT(B2:B7)</f>
+        <v/>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(B2:B7)</f>
+        <v/>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(C2:C7)</f>
+        <v/>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(D2:D7)</f>
+        <v/>
+      </c>
+      <c r="E8">
+        <f>AVERAGE(E2:E7)</f>
+        <v/>
+      </c>
+      <c r="F8">
+        <f>AVERAGE(F2:F7)</f>
+        <v/>
+      </c>
+      <c r="G8">
+        <f>AVERAGE(G2:G7)</f>
+        <v/>
+      </c>
+      <c r="H8">
+        <f>AVERAGE(H2:H7)</f>
+        <v/>
+      </c>
+      <c r="I8">
+        <f>AVERAGE(I2:I7)</f>
+        <v/>
+      </c>
+      <c r="J8">
+        <f>AVERAGE(J2:J7)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="65" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp44307.0_20242011_125146.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp76088.0_20242011_125250.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp21366.0_20242011_125533.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp21366.0_20242011_125650.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp37077.0_20242011_125625.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp28238.0_20242011_125426.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp51299.0_20242011_125355.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp188553.0_20242011_125739.png</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>11.33</v>
+      </c>
+      <c r="C9" t="n">
+        <v>14.15</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-45.39</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="F9" t="n">
+        <v>14.21</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="I9" t="n">
+        <v>11.49</v>
+      </c>
+      <c r="J9" t="n">
+        <v>5.62</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <f>COUNT(B2:B9)</f>
+        <v/>
+      </c>
+      <c r="B10">
+        <f>AVERAGE(B2:B9)</f>
+        <v/>
+      </c>
+      <c r="C10">
+        <f>AVERAGE(C2:C9)</f>
+        <v/>
+      </c>
+      <c r="D10">
+        <f>AVERAGE(D2:D9)</f>
+        <v/>
+      </c>
+      <c r="E10">
+        <f>AVERAGE(E2:E9)</f>
+        <v/>
+      </c>
+      <c r="F10">
+        <f>AVERAGE(F2:F9)</f>
+        <v/>
+      </c>
+      <c r="G10">
+        <f>AVERAGE(G2:G9)</f>
+        <v/>
+      </c>
+      <c r="H10">
+        <f>AVERAGE(H2:H9)</f>
+        <v/>
+      </c>
+      <c r="I10">
+        <f>AVERAGE(I2:I9)</f>
+        <v/>
+      </c>
+      <c r="J10">
+        <f>AVERAGE(J2:J9)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="65" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp29589.0_20242011_130019.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp38487.0_20242011_130056.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp20194.0_20242011_130422.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp34356.0_20242011_130346.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp31138.0_20242011_130209.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp55033.0_20242011_130245.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp155421.0_20242011_130527.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <f>COUNT(B2:B8)</f>
+        <v/>
+      </c>
+      <c r="B9">
+        <f>AVERAGE(B2:B8)</f>
+        <v/>
+      </c>
+      <c r="C9">
+        <f>AVERAGE(C2:C8)</f>
+        <v/>
+      </c>
+      <c r="D9">
+        <f>AVERAGE(D2:D8)</f>
+        <v/>
+      </c>
+      <c r="E9">
+        <f>AVERAGE(E2:E8)</f>
+        <v/>
+      </c>
+      <c r="F9">
+        <f>AVERAGE(F2:F8)</f>
+        <v/>
+      </c>
+      <c r="G9">
+        <f>AVERAGE(G2:G8)</f>
+        <v/>
+      </c>
+      <c r="H9">
+        <f>AVERAGE(H2:H8)</f>
+        <v/>
+      </c>
+      <c r="I9">
+        <f>AVERAGE(I2:I8)</f>
+        <v/>
+      </c>
+      <c r="J9">
+        <f>AVERAGE(J2:J8)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="69" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp25100.0_20242011_130817.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp48300.0_20242011_131100.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp62482.0_20242011_130903.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp79087.0_20242011_131136.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp21306.0_20242011_131253.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp37435.0_20242011_131220.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp28973.0_20242011_131020.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp47267.0_20242011_130950.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightCLOSE_exp189824.0_20242011_131447.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp169067.0_20242011_131356.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <f>COUNT(B2:B11)</f>
+        <v/>
+      </c>
+      <c r="B12">
+        <f>AVERAGE(B2:B11)</f>
+        <v/>
+      </c>
+      <c r="C12">
+        <f>AVERAGE(C2:C11)</f>
+        <v/>
+      </c>
+      <c r="D12">
+        <f>AVERAGE(D2:D11)</f>
+        <v/>
+      </c>
+      <c r="E12">
+        <f>AVERAGE(E2:E11)</f>
+        <v/>
+      </c>
+      <c r="F12">
+        <f>AVERAGE(F2:F11)</f>
+        <v/>
+      </c>
+      <c r="G12">
+        <f>AVERAGE(G2:G11)</f>
+        <v/>
+      </c>
+      <c r="H12">
+        <f>AVERAGE(H2:H11)</f>
+        <v/>
+      </c>
+      <c r="I12">
+        <f>AVERAGE(I2:I11)</f>
+        <v/>
+      </c>
+      <c r="J12">
+        <f>AVERAGE(J2:J11)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="66" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp32131.0_20242011_134258.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp55848.0_20242011_134226.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp25716.0_20242011_134400.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp45718.0_20242011_134436.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp27007.0_20242011_134020.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp51458.0_20242011_134118.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Two_light_Pallet_half_way_light10_exp10282.0_20242011_133038.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp174946.0_20242011_134540.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <f>COUNT(B2:B9)</f>
+        <v/>
+      </c>
+      <c r="B10">
+        <f>AVERAGE(B2:B9)</f>
+        <v/>
+      </c>
+      <c r="C10">
+        <f>AVERAGE(C2:C9)</f>
+        <v/>
+      </c>
+      <c r="D10">
+        <f>AVERAGE(D2:D9)</f>
+        <v/>
+      </c>
+      <c r="E10">
+        <f>AVERAGE(E2:E9)</f>
+        <v/>
+      </c>
+      <c r="F10">
+        <f>AVERAGE(F2:F9)</f>
+        <v/>
+      </c>
+      <c r="G10">
+        <f>AVERAGE(G2:G9)</f>
+        <v/>
+      </c>
+      <c r="H10">
+        <f>AVERAGE(H2:H9)</f>
+        <v/>
+      </c>
+      <c r="I10">
+        <f>AVERAGE(I2:I9)</f>
+        <v/>
+      </c>
+      <c r="J10">
+        <f>AVERAGE(J2:J9)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -494,13 +1965,13 @@
         <v>9.619999999999999</v>
       </c>
       <c r="C2" t="n">
-        <v>14.41</v>
+        <v>14.4</v>
       </c>
       <c r="D2" t="n">
         <v>6.07</v>
       </c>
       <c r="E2" t="n">
-        <v>4.58</v>
+        <v>4.59</v>
       </c>
       <c r="F2" t="n">
         <v>20.21</v>
@@ -524,6 +1995,33 @@
           <t>Beside_Camera_light5_20242011_094046.png</t>
         </is>
       </c>
+      <c r="B3" t="n">
+        <v>7.94</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11.71</v>
+      </c>
+      <c r="D3" t="n">
+        <v>13.03</v>
+      </c>
+      <c r="E3" t="n">
+        <v>5.27</v>
+      </c>
+      <c r="F3" t="n">
+        <v>22.58</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3.42</v>
+      </c>
+      <c r="I3" t="n">
+        <v>17.24</v>
+      </c>
+      <c r="J3" t="n">
+        <v>4.11</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -546,16 +2044,16 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>12.66</v>
+        <v>12.49</v>
       </c>
       <c r="C6" t="n">
-        <v>14.61</v>
+        <v>14</v>
       </c>
       <c r="D6" t="n">
         <v>-4.13</v>
       </c>
       <c r="E6" t="n">
-        <v>5.59</v>
+        <v>5.63</v>
       </c>
       <c r="F6" t="n">
         <v>16.14</v>
@@ -567,7 +2065,7 @@
         <v>7.73</v>
       </c>
       <c r="I6" t="n">
-        <v>13.98</v>
+        <v>13.93</v>
       </c>
       <c r="J6" t="n">
         <v>8.24</v>
@@ -580,16 +2078,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>9.17</v>
+        <v>9.15</v>
       </c>
       <c r="C7" t="n">
-        <v>14.63</v>
+        <v>14.17</v>
       </c>
       <c r="D7" t="n">
         <v>8.539999999999999</v>
       </c>
       <c r="E7" t="n">
-        <v>3.57</v>
+        <v>3.55</v>
       </c>
       <c r="F7" t="n">
         <v>21</v>
@@ -601,13 +2099,17 @@
         <v>4.79</v>
       </c>
       <c r="I7" t="n">
-        <v>17.52</v>
+        <v>17.51</v>
       </c>
       <c r="J7" t="n">
         <v>5.51</v>
       </c>
     </row>
     <row r="8">
+      <c r="A8">
+        <f>COUNT(B2:B7)</f>
+        <v/>
+      </c>
       <c r="B8">
         <f>AVERAGE(B2:B7)</f>
         <v/>
@@ -646,6 +2148,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>